<commit_message>
BOM v1 MS, à faire verif par MPL
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
+++ b/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\MS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2019\CR - Cost Report\BOM\MS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3DDBBA-CE6E-45EB-BFAA-4869D05A1AE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>System</t>
   </si>
@@ -57,9 +63,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name of the part</t>
-  </si>
-  <si>
     <t>m or b</t>
   </si>
   <si>
@@ -117,27 +120,12 @@
     <t>MS_01005</t>
   </si>
   <si>
-    <t>MS_01006</t>
-  </si>
-  <si>
     <t>MS_02001</t>
   </si>
   <si>
     <t>MS_02002</t>
   </si>
   <si>
-    <t>MS_02003</t>
-  </si>
-  <si>
-    <t>MS_02004</t>
-  </si>
-  <si>
-    <t>MS_02005</t>
-  </si>
-  <si>
-    <t>MS_02006</t>
-  </si>
-  <si>
     <t>Driver's harness</t>
   </si>
   <si>
@@ -156,12 +144,6 @@
     <t>MS_03004</t>
   </si>
   <si>
-    <t>MS_03005</t>
-  </si>
-  <si>
-    <t>MS_03006</t>
-  </si>
-  <si>
     <t>MS_A0400</t>
   </si>
   <si>
@@ -177,19 +159,73 @@
     <t>MS_04003</t>
   </si>
   <si>
-    <t>MS_04004</t>
-  </si>
-  <si>
-    <t>MS_04005</t>
-  </si>
-  <si>
-    <t>MS_04006</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Firewall Bottom Plate</t>
+  </si>
+  <si>
+    <t>Firewall Main Plate</t>
+  </si>
+  <si>
+    <t>Firewall Top Plate</t>
+  </si>
+  <si>
+    <t>Mousse Epaules</t>
+  </si>
+  <si>
+    <t>Mousse Longue</t>
+  </si>
+  <si>
+    <t>Seat</t>
+  </si>
+  <si>
+    <t>Lower Seat Tabs</t>
+  </si>
+  <si>
+    <t>Back Seat Tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Low Harness Tab</t>
+  </si>
+  <si>
+    <t>Headrest Plate</t>
+  </si>
+  <si>
+    <t>Headrest Bracket</t>
+  </si>
+  <si>
+    <t>Pas indique, a verif avec MPL</t>
+  </si>
+  <si>
+    <t>Ailettes ? Pas vu sur la maquette, ni en vrai</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Upper Harness Tab ? Non indiqué par Yohan, pas sur la maquette, et en vrai ?</t>
+  </si>
+  <si>
+    <t>Mettre les mousses dans le BOM ?</t>
+  </si>
+  <si>
+    <t>Firewall Tabs</t>
+  </si>
+  <si>
+    <t>Commentaires pour MPL :</t>
+  </si>
+  <si>
+    <t>Nomenclature non respecté pour Headrest (A0300-&gt;A0200 et Driver Harness : A0500-&gt;A0300 car il n'y a pas de rollbar padding, cest grave ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 ? Que 1 sur la maquette </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -260,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -294,11 +330,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -310,6 +355,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -591,12 +642,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,9 +660,10 @@
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +671,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -634,293 +686,298 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F14" s="4">
+        <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="E15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>31</v>
@@ -930,16 +987,16 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>32</v>
@@ -949,205 +1006,19 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modif Cost MS+ Finalisation Pare Feu
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
+++ b/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2019\CR - Cost Report\BOM\MS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3DDBBA-CE6E-45EB-BFAA-4869D05A1AE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95635695-759D-41F5-B707-9CFBF626C7A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>System</t>
   </si>
@@ -63,13 +63,7 @@
     <t>ID</t>
   </si>
   <si>
-    <t>m or b</t>
-  </si>
-  <si>
     <t>Short description of the part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number </t>
   </si>
   <si>
     <t>FR</t>
@@ -123,9 +117,6 @@
     <t>MS_02001</t>
   </si>
   <si>
-    <t>MS_02002</t>
-  </si>
-  <si>
     <t>Driver's harness</t>
   </si>
   <si>
@@ -138,12 +129,6 @@
     <t>MS_03002</t>
   </si>
   <si>
-    <t>MS_03003</t>
-  </si>
-  <si>
-    <t>MS_03004</t>
-  </si>
-  <si>
     <t>MS_A0400</t>
   </si>
   <si>
@@ -153,12 +138,6 @@
     <t>MS_04001</t>
   </si>
   <si>
-    <t>MS_04002</t>
-  </si>
-  <si>
-    <t>MS_04003</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -171,55 +150,55 @@
     <t>Firewall Top Plate</t>
   </si>
   <si>
-    <t>Mousse Epaules</t>
-  </si>
-  <si>
-    <t>Mousse Longue</t>
-  </si>
-  <si>
     <t>Seat</t>
   </si>
   <si>
-    <t>Lower Seat Tabs</t>
-  </si>
-  <si>
-    <t>Back Seat Tabs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Low Harness Tab</t>
-  </si>
-  <si>
     <t>Headrest Plate</t>
   </si>
   <si>
-    <t>Headrest Bracket</t>
-  </si>
-  <si>
-    <t>Pas indique, a verif avec MPL</t>
-  </si>
-  <si>
-    <t>Ailettes ? Pas vu sur la maquette, ni en vrai</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Upper Harness Tab ? Non indiqué par Yohan, pas sur la maquette, et en vrai ?</t>
-  </si>
-  <si>
-    <t>Mettre les mousses dans le BOM ?</t>
-  </si>
-  <si>
-    <t>Firewall Tabs</t>
-  </si>
-  <si>
-    <t>Commentaires pour MPL :</t>
-  </si>
-  <si>
-    <t>Nomenclature non respecté pour Headrest (A0300-&gt;A0200 et Driver Harness : A0500-&gt;A0300 car il n'y a pas de rollbar padding, cest grave ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 ? Que 1 sur la maquette </t>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Mise en plan ?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Firewall Joints</t>
+  </si>
+  <si>
+    <t>Join the two parts of the Firewall Top Plate</t>
+  </si>
+  <si>
+    <t>Protect the pilote from behind</t>
+  </si>
+  <si>
+    <t>Protect the pilote from the middle</t>
+  </si>
+  <si>
+    <t>Protect the pilote from the top</t>
+  </si>
+  <si>
+    <t>Short Shoulders Foam</t>
+  </si>
+  <si>
+    <t>Long Shoulders Foam</t>
+  </si>
+  <si>
+    <t>Firewall Middle Floor Plate</t>
+  </si>
+  <si>
+    <t>Firewall Side Floor Plate</t>
+  </si>
+  <si>
+    <t>MS_01006</t>
+  </si>
+  <si>
+    <t>Join the Firewall to the Floor Pan</t>
+  </si>
+  <si>
+    <t>Sthrengthen the Headrest</t>
   </si>
 </sst>
 </file>
@@ -643,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -688,337 +667,268 @@
     </row>
     <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>52</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="199.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>8</v>
+      <c r="F15" s="4">
+        <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="4">
-        <v>4</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="4">
-        <v>2</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost MS, ergo mal rangé/pas fini ptin
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
+++ b/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2019\CR - Cost Report\BOM\MS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95635695-759D-41F5-B707-9CFBF626C7A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC96F6E3-9678-4EFC-9978-42E35D4E1C1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>System</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Short description of the part</t>
-  </si>
-  <si>
     <t>FR</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>Mise en plan ?</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -199,6 +193,45 @@
   </si>
   <si>
     <t>Sthrengthen the Headrest</t>
+  </si>
+  <si>
+    <t>Harness</t>
+  </si>
+  <si>
+    <t>Seatbelt of the Pilote</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Compressé</t>
+  </si>
+  <si>
+    <t>MEP</t>
+  </si>
+  <si>
+    <t>Back Foam</t>
+  </si>
+  <si>
+    <t>MS_03004</t>
+  </si>
+  <si>
+    <t>MS_04002</t>
+  </si>
+  <si>
+    <t>Side Head Foam</t>
+  </si>
+  <si>
+    <t>MS_02002</t>
+  </si>
+  <si>
+    <t>Head Foam</t>
+  </si>
+  <si>
+    <t>MS_02003</t>
+  </si>
+  <si>
+    <t>Inutile</t>
   </si>
 </sst>
 </file>
@@ -249,7 +282,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +304,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4A7D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,12 +375,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,27 +659,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="45.88671875" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -664,275 +703,462 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4">
         <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4">
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Une Ref erronée sur BOM MS
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
+++ b/CR - Cost Report/BOM/MS/MSA0100_to_MSA0400.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\MS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2019\CR - Cost Report\BOM\MS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4CB898-04E2-4CC1-AB7E-F1A6C17348DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,11 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -212,9 +208,6 @@
     <t>Back Foam</t>
   </si>
   <si>
-    <t>MS_03004</t>
-  </si>
-  <si>
     <t>MS_04002</t>
   </si>
   <si>
@@ -249,12 +242,15 @@
   </si>
   <si>
     <t>Soften the contact for the back</t>
+  </si>
+  <si>
+    <t>MS_03003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -675,12 +671,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +690,7 @@
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -885,7 +881,7 @@
         <v>33</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -913,7 +909,7 @@
         <v>33</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -959,26 +955,26 @@
         <v>33</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>33</v>
@@ -987,35 +983,35 @@
         <v>33</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1046,7 +1042,7 @@
         <v>26</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1061,7 +1057,7 @@
         <v>33</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1074,7 +1070,7 @@
         <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
@@ -1089,7 +1085,7 @@
         <v>33</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1108,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>33</v>
@@ -1117,7 +1113,7 @@
         <v>33</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1161,7 +1157,7 @@
         <v>33</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1174,13 +1170,13 @@
         <v>26</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>33</v>
@@ -1189,7 +1185,7 @@
         <v>33</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>